<commit_message>
Modelo corriendo a 5 temporadas
</commit_message>
<xml_diff>
--- a/Parametros_Finales.xlsx
+++ b/Parametros_Finales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pedroirarrazaval/Desktop/Modelo-Capstone/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48213EF4-9D8A-E64E-B6BE-75637381A060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{458BCDC4-08A0-BF4C-9C27-C4302FABCC7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12460" yWindow="500" windowWidth="16340" windowHeight="17500" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12460" yWindow="500" windowWidth="16340" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Índices" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="114">
   <si>
     <t>Centrales</t>
   </si>
@@ -320,9 +320,6 @@
     <t>psi</t>
   </si>
   <si>
-    <t>MWh</t>
-  </si>
-  <si>
     <t>phi</t>
   </si>
   <si>
@@ -381,6 +378,18 @@
   </si>
   <si>
     <t>t</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>m3/s</t>
+  </si>
+  <si>
+    <t>V_MIN</t>
+  </si>
+  <si>
+    <t>GWh</t>
   </si>
 </sst>
 </file>
@@ -696,21 +705,6 @@
     <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -734,6 +728,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1280,14 +1289,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="39"/>
-      <c r="D1" s="36" t="s">
+      <c r="A1" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="45"/>
+      <c r="D1" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="37"/>
+      <c r="E1" s="47"/>
       <c r="F1" s="8"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1347,10 +1356,10 @@
       <c r="B6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="36" t="s">
+      <c r="D6" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="37"/>
+      <c r="E6" s="47"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
@@ -1395,10 +1404,10 @@
       <c r="B10" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="36" t="s">
+      <c r="D10" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="37"/>
+      <c r="E10" s="47"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
@@ -1457,10 +1466,10 @@
       <c r="B15" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="36" t="s">
+      <c r="D15" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="E15" s="37"/>
+      <c r="E15" s="47"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
@@ -1500,10 +1509,10 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="38" t="s">
-        <v>95</v>
-      </c>
-      <c r="B19" s="38"/>
+      <c r="A19" s="48" t="s">
+        <v>94</v>
+      </c>
+      <c r="B19" s="48"/>
       <c r="D19" s="6">
         <v>4</v>
       </c>
@@ -1536,7 +1545,7 @@
         <v>6</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -1554,10 +1563,10 @@
       <c r="B23" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="D23" s="36" t="s">
-        <v>97</v>
-      </c>
-      <c r="E23" s="37"/>
+      <c r="D23" s="46" t="s">
+        <v>96</v>
+      </c>
+      <c r="E23" s="47"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
@@ -2184,10 +2193,10 @@
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A69" s="38" t="s">
-        <v>102</v>
-      </c>
-      <c r="B69" s="38"/>
+      <c r="A69" s="48" t="s">
+        <v>101</v>
+      </c>
+      <c r="B69" s="48"/>
       <c r="D69" s="14">
         <v>46</v>
       </c>
@@ -2200,7 +2209,7 @@
         <v>1</v>
       </c>
       <c r="B70" s="32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D70" s="14">
         <v>47</v>
@@ -2214,7 +2223,7 @@
         <v>2</v>
       </c>
       <c r="B71" s="32" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D71" s="14">
         <v>48</v>
@@ -2228,7 +2237,7 @@
         <v>3</v>
       </c>
       <c r="B72" s="32" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D72" s="14">
         <v>49</v>
@@ -2242,7 +2251,7 @@
         <v>4</v>
       </c>
       <c r="B73" s="32" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D73" s="14">
         <v>50</v>
@@ -2256,7 +2265,7 @@
         <v>5</v>
       </c>
       <c r="B74" s="32" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D74" s="14">
         <v>51</v>
@@ -2483,14 +2492,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D10:E10"/>
     <mergeCell ref="A69:B69"/>
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="D23:E23"/>
     <mergeCell ref="D6:E6"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="D10:E10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2500,7 +2509,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC4D74B6-4A46-4CB3-9332-532A38679EE3}">
   <dimension ref="A1:B49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
@@ -2508,10 +2517,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="29" t="s">
         <v>92</v>
-      </c>
-      <c r="B1" s="29" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -2905,10 +2914,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AB113F6-B42D-7F43-8024-ED9A3F5718C9}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2920,19 +2929,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="37"/>
-      <c r="E1" s="39" t="s">
-        <v>98</v>
-      </c>
-      <c r="F1" s="39"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="47"/>
+      <c r="E1" s="45" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" s="45"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B2" s="6">
         <v>4800</v>
@@ -2949,7 +2958,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B3" s="6">
         <v>5000</v>
@@ -2966,10 +2975,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>28</v>
+        <v>112</v>
       </c>
       <c r="B4" s="6">
-        <v>5582</v>
+        <v>1400</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>27</v>
@@ -2983,12 +2992,14 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>99</v>
+        <v>28</v>
       </c>
       <c r="B5" s="6">
-        <v>4</v>
-      </c>
-      <c r="C5" s="6"/>
+        <v>5582</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>27</v>
+      </c>
       <c r="E5" s="6">
         <v>4</v>
       </c>
@@ -2998,35 +3009,55 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B6" s="6">
-        <v>1</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>101</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="C6" s="6"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="B7" s="6">
-        <v>1000000000</v>
+        <v>1</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B8" s="6">
-        <v>1000000000</v>
+        <v>1000</v>
       </c>
       <c r="C8" s="6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
         <v>90</v>
+      </c>
+      <c r="B9" s="6">
+        <v>1000</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B10" s="6">
+        <v>1000</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -5475,14 +5506,14 @@
   <dimension ref="A1:AX32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+      <selection activeCell="A8" sqref="A3:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A1" s="31" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B1" s="31" t="s">
         <v>34</v>
@@ -5634,7 +5665,7 @@
     </row>
     <row r="2" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A2" s="31" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B2" s="31" t="s">
         <v>83</v>
@@ -8521,10 +8552,10 @@
       </c>
     </row>
     <row r="21" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A21" s="41">
+      <c r="A21" s="36">
         <v>4</v>
       </c>
-      <c r="B21" s="42" t="s">
+      <c r="B21" s="37" t="s">
         <v>2</v>
       </c>
       <c r="C21" s="34">
@@ -8673,770 +8704,770 @@
       </c>
     </row>
     <row r="22" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A22" s="43">
+      <c r="A22" s="38">
         <v>4</v>
       </c>
-      <c r="B22" s="44" t="s">
+      <c r="B22" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="C22" s="45">
+      <c r="C22" s="40">
         <v>0.30380000000000001</v>
       </c>
-      <c r="D22" s="45">
+      <c r="D22" s="40">
         <v>0.33550000000000002</v>
       </c>
-      <c r="E22" s="45">
+      <c r="E22" s="40">
         <v>0.33329999999999999</v>
       </c>
-      <c r="F22" s="45">
+      <c r="F22" s="40">
         <v>0.57740000000000002</v>
       </c>
-      <c r="G22" s="45">
+      <c r="G22" s="40">
         <v>1.2271000000000001</v>
       </c>
-      <c r="H22" s="45">
+      <c r="H22" s="40">
         <v>0.99550000000000005</v>
       </c>
-      <c r="I22" s="45">
+      <c r="I22" s="40">
         <v>1.2551000000000001</v>
       </c>
-      <c r="J22" s="45">
+      <c r="J22" s="40">
         <v>3.5543999999999998</v>
       </c>
-      <c r="K22" s="45">
+      <c r="K22" s="40">
         <v>6.2462</v>
       </c>
-      <c r="L22" s="45">
+      <c r="L22" s="40">
         <v>8.4306999999999999</v>
       </c>
-      <c r="M22" s="45">
+      <c r="M22" s="40">
         <v>3.9758</v>
       </c>
-      <c r="N22" s="45">
+      <c r="N22" s="40">
         <v>46.954700000000003</v>
       </c>
-      <c r="O22" s="45">
+      <c r="O22" s="40">
         <v>15.176</v>
       </c>
-      <c r="P22" s="45">
+      <c r="P22" s="40">
         <v>10.0284</v>
       </c>
-      <c r="Q22" s="45">
+      <c r="Q22" s="40">
         <v>9.2880000000000003</v>
       </c>
-      <c r="R22" s="45">
+      <c r="R22" s="40">
         <v>9.8729999999999993</v>
       </c>
-      <c r="S22" s="45">
+      <c r="S22" s="40">
         <v>8.5383999999999993</v>
       </c>
-      <c r="T22" s="45">
+      <c r="T22" s="40">
         <v>7.0475000000000003</v>
       </c>
-      <c r="U22" s="45">
+      <c r="U22" s="40">
         <v>28.213899999999999</v>
       </c>
-      <c r="V22" s="45">
+      <c r="V22" s="40">
         <v>16.5334</v>
       </c>
-      <c r="W22" s="45">
+      <c r="W22" s="40">
         <v>9.8302999999999994</v>
       </c>
-      <c r="X22" s="45">
+      <c r="X22" s="40">
         <v>9.7766999999999999</v>
       </c>
-      <c r="Y22" s="45">
+      <c r="Y22" s="40">
         <v>9.7760999999999996</v>
       </c>
-      <c r="Z22" s="45">
+      <c r="Z22" s="40">
         <v>5.6445999999999996</v>
       </c>
-      <c r="AA22" s="45">
+      <c r="AA22" s="40">
         <v>4.9169999999999998</v>
       </c>
-      <c r="AB22" s="45">
+      <c r="AB22" s="40">
         <v>4.3285</v>
       </c>
-      <c r="AC22" s="45">
+      <c r="AC22" s="40">
         <v>6.1745000000000001</v>
       </c>
-      <c r="AD22" s="45">
+      <c r="AD22" s="40">
         <v>7.7904999999999998</v>
       </c>
-      <c r="AE22" s="45">
+      <c r="AE22" s="40">
         <v>6.7957000000000001</v>
       </c>
-      <c r="AF22" s="45">
+      <c r="AF22" s="40">
         <v>7.8418999999999999</v>
       </c>
-      <c r="AG22" s="45">
+      <c r="AG22" s="40">
         <v>8.4492999999999991</v>
       </c>
-      <c r="AH22" s="45">
+      <c r="AH22" s="40">
         <v>9.7650000000000006</v>
       </c>
-      <c r="AI22" s="45">
+      <c r="AI22" s="40">
         <v>6.3874000000000004</v>
       </c>
-      <c r="AJ22" s="45">
+      <c r="AJ22" s="40">
         <v>5.8741000000000003</v>
       </c>
-      <c r="AK22" s="45">
+      <c r="AK22" s="40">
         <v>4.6536999999999997</v>
       </c>
-      <c r="AL22" s="45">
+      <c r="AL22" s="40">
         <v>4.0388999999999999</v>
       </c>
-      <c r="AM22" s="45">
+      <c r="AM22" s="40">
         <v>2.8151000000000002</v>
       </c>
-      <c r="AN22" s="45">
+      <c r="AN22" s="40">
         <v>3.7141000000000002</v>
       </c>
-      <c r="AO22" s="45">
+      <c r="AO22" s="40">
         <v>4.0777000000000001</v>
       </c>
-      <c r="AP22" s="45">
+      <c r="AP22" s="40">
         <v>4.4039999999999999</v>
       </c>
-      <c r="AQ22" s="45">
+      <c r="AQ22" s="40">
         <v>3.7584</v>
       </c>
-      <c r="AR22" s="45">
+      <c r="AR22" s="40">
         <v>4.1703999999999999</v>
       </c>
-      <c r="AS22" s="45">
+      <c r="AS22" s="40">
         <v>3.5545</v>
       </c>
-      <c r="AT22" s="45">
+      <c r="AT22" s="40">
         <v>3.5249999999999999</v>
       </c>
-      <c r="AU22" s="45">
+      <c r="AU22" s="40">
         <v>2.6757</v>
       </c>
-      <c r="AV22" s="45">
+      <c r="AV22" s="40">
         <v>2.6162999999999998</v>
       </c>
-      <c r="AW22" s="45">
+      <c r="AW22" s="40">
         <v>1.7538</v>
       </c>
-      <c r="AX22" s="45">
+      <c r="AX22" s="40">
         <v>1.9450000000000001</v>
       </c>
     </row>
     <row r="23" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A23" s="43">
+      <c r="A23" s="38">
         <v>4</v>
       </c>
-      <c r="B23" s="44" t="s">
+      <c r="B23" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="45">
+      <c r="C23" s="40">
         <v>7.9802999999999997</v>
       </c>
-      <c r="D23" s="45">
+      <c r="D23" s="40">
         <v>7.6040999999999999</v>
       </c>
-      <c r="E23" s="45">
+      <c r="E23" s="40">
         <v>7.5530999999999997</v>
       </c>
-      <c r="F23" s="45">
+      <c r="F23" s="40">
         <v>13.176500000000001</v>
       </c>
-      <c r="G23" s="45">
+      <c r="G23" s="40">
         <v>12.1896</v>
       </c>
-      <c r="H23" s="45">
+      <c r="H23" s="40">
         <v>9.8892000000000007</v>
       </c>
-      <c r="I23" s="45">
+      <c r="I23" s="40">
         <v>12.4674</v>
       </c>
-      <c r="J23" s="45">
+      <c r="J23" s="40">
         <v>35.308199999999999</v>
       </c>
-      <c r="K23" s="45">
+      <c r="K23" s="40">
         <v>62.047699999999999</v>
       </c>
-      <c r="L23" s="45">
+      <c r="L23" s="40">
         <v>83.747799999999998</v>
       </c>
-      <c r="M23" s="45">
+      <c r="M23" s="40">
         <v>39.494199999999999</v>
       </c>
-      <c r="N23" s="45">
+      <c r="N23" s="40">
         <v>466.43060000000003</v>
       </c>
-      <c r="O23" s="45">
+      <c r="O23" s="40">
         <v>150.7527</v>
       </c>
-      <c r="P23" s="45">
+      <c r="P23" s="40">
         <v>99.618600000000001</v>
       </c>
-      <c r="Q23" s="45">
+      <c r="Q23" s="40">
         <v>92.263400000000004</v>
       </c>
-      <c r="R23" s="45">
+      <c r="R23" s="40">
         <v>98.0745</v>
       </c>
-      <c r="S23" s="45">
+      <c r="S23" s="40">
         <v>84.816999999999993</v>
       </c>
-      <c r="T23" s="45">
+      <c r="T23" s="40">
         <v>70.007300000000001</v>
       </c>
-      <c r="U23" s="45">
+      <c r="U23" s="40">
         <v>280.26679999999999</v>
       </c>
-      <c r="V23" s="45">
+      <c r="V23" s="40">
         <v>164.23670000000001</v>
       </c>
-      <c r="W23" s="45">
+      <c r="W23" s="40">
         <v>131.8903</v>
       </c>
-      <c r="X23" s="45">
+      <c r="X23" s="40">
         <v>186.15350000000001</v>
       </c>
-      <c r="Y23" s="45">
+      <c r="Y23" s="40">
         <v>186.14359999999999</v>
       </c>
-      <c r="Z23" s="45">
+      <c r="Z23" s="40">
         <v>112.143</v>
       </c>
-      <c r="AA23" s="45">
+      <c r="AA23" s="40">
         <v>95.753799999999998</v>
       </c>
-      <c r="AB23" s="45">
+      <c r="AB23" s="40">
         <v>84.281400000000005</v>
       </c>
-      <c r="AC23" s="45">
+      <c r="AC23" s="40">
         <v>90.786000000000001</v>
       </c>
-      <c r="AD23" s="45">
+      <c r="AD23" s="40">
         <v>104.1803</v>
       </c>
-      <c r="AE23" s="45">
+      <c r="AE23" s="40">
         <v>102.56100000000001</v>
       </c>
-      <c r="AF23" s="45">
+      <c r="AF23" s="40">
         <v>105.1374</v>
       </c>
-      <c r="AG23" s="45">
+      <c r="AG23" s="40">
         <v>115.3991</v>
       </c>
-      <c r="AH23" s="45">
+      <c r="AH23" s="40">
         <v>133.2433</v>
       </c>
-      <c r="AI23" s="45">
+      <c r="AI23" s="40">
         <v>112.6189</v>
       </c>
-      <c r="AJ23" s="45">
+      <c r="AJ23" s="40">
         <v>94.846800000000002</v>
       </c>
-      <c r="AK23" s="45">
+      <c r="AK23" s="40">
         <v>74.649699999999996</v>
       </c>
-      <c r="AL23" s="45">
+      <c r="AL23" s="40">
         <v>63.080500000000001</v>
       </c>
-      <c r="AM23" s="45">
+      <c r="AM23" s="40">
         <v>49.628599999999999</v>
       </c>
-      <c r="AN23" s="45">
+      <c r="AN23" s="40">
         <v>42.404299999999999</v>
       </c>
-      <c r="AO23" s="45">
+      <c r="AO23" s="40">
         <v>37.862099999999998</v>
       </c>
-      <c r="AP23" s="45">
+      <c r="AP23" s="40">
         <v>32.775399999999998</v>
       </c>
-      <c r="AQ23" s="45">
+      <c r="AQ23" s="40">
         <v>29.386700000000001</v>
       </c>
-      <c r="AR23" s="45">
+      <c r="AR23" s="40">
         <v>27.220500000000001</v>
       </c>
-      <c r="AS23" s="45">
+      <c r="AS23" s="40">
         <v>25.061699999999998</v>
       </c>
-      <c r="AT23" s="45">
+      <c r="AT23" s="40">
         <v>22.666399999999999</v>
       </c>
-      <c r="AU23" s="45">
+      <c r="AU23" s="40">
         <v>19.9833</v>
       </c>
-      <c r="AV23" s="45">
+      <c r="AV23" s="40">
         <v>18.886299999999999</v>
       </c>
-      <c r="AW23" s="45">
+      <c r="AW23" s="40">
         <v>19.750699999999998</v>
       </c>
-      <c r="AX23" s="45">
+      <c r="AX23" s="40">
         <v>18.032399999999999</v>
       </c>
     </row>
     <row r="24" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A24" s="43">
+      <c r="A24" s="38">
         <v>4</v>
       </c>
-      <c r="B24" s="44" t="s">
+      <c r="B24" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="45">
+      <c r="C24" s="40">
         <v>24.087800000000001</v>
       </c>
-      <c r="D24" s="45">
+      <c r="D24" s="40">
         <v>24.008700000000001</v>
       </c>
-      <c r="E24" s="45">
+      <c r="E24" s="40">
         <v>19.410900000000002</v>
       </c>
-      <c r="F24" s="45">
+      <c r="F24" s="40">
         <v>20.5943</v>
       </c>
-      <c r="G24" s="45">
+      <c r="G24" s="40">
         <v>18.503900000000002</v>
       </c>
-      <c r="H24" s="45">
+      <c r="H24" s="40">
         <v>15.536300000000001</v>
       </c>
-      <c r="I24" s="45">
+      <c r="I24" s="40">
         <v>29.118099999999998</v>
       </c>
-      <c r="J24" s="45">
+      <c r="J24" s="40">
         <v>49.311399999999999</v>
       </c>
-      <c r="K24" s="45">
+      <c r="K24" s="40">
         <v>57.905799999999999</v>
       </c>
-      <c r="L24" s="45">
+      <c r="L24" s="40">
         <v>95.133099999999999</v>
       </c>
-      <c r="M24" s="45">
+      <c r="M24" s="40">
         <v>20.4483</v>
       </c>
-      <c r="N24" s="45">
+      <c r="N24" s="40">
         <v>311.5539</v>
       </c>
-      <c r="O24" s="45">
+      <c r="O24" s="40">
         <v>69.771000000000001</v>
       </c>
-      <c r="P24" s="45">
+      <c r="P24" s="40">
         <v>11.9916</v>
       </c>
-      <c r="Q24" s="45">
+      <c r="Q24" s="40">
         <v>29.9984</v>
       </c>
-      <c r="R24" s="45">
+      <c r="R24" s="40">
         <v>105.80710000000001</v>
       </c>
-      <c r="S24" s="45">
+      <c r="S24" s="40">
         <v>75.442899999999995</v>
       </c>
-      <c r="T24" s="45">
+      <c r="T24" s="40">
         <v>56.216500000000003</v>
       </c>
-      <c r="U24" s="45">
+      <c r="U24" s="40">
         <v>260.79180000000002</v>
       </c>
-      <c r="V24" s="45">
+      <c r="V24" s="40">
         <v>95.894900000000007</v>
       </c>
-      <c r="W24" s="45">
+      <c r="W24" s="40">
         <v>58.996899999999997</v>
       </c>
-      <c r="X24" s="45">
+      <c r="X24" s="40">
         <v>121.681</v>
       </c>
-      <c r="Y24" s="45">
+      <c r="Y24" s="40">
         <v>165.72890000000001</v>
       </c>
-      <c r="Z24" s="45">
+      <c r="Z24" s="40">
         <v>44.283200000000001</v>
       </c>
-      <c r="AA24" s="45">
+      <c r="AA24" s="40">
         <v>23.104800000000001</v>
       </c>
-      <c r="AB24" s="45">
-        <v>0</v>
-      </c>
-      <c r="AC24" s="45">
-        <v>0</v>
-      </c>
-      <c r="AD24" s="45">
-        <v>0</v>
-      </c>
-      <c r="AE24" s="45">
-        <v>0</v>
-      </c>
-      <c r="AF24" s="45">
-        <v>0</v>
-      </c>
-      <c r="AG24" s="45">
-        <v>0</v>
-      </c>
-      <c r="AH24" s="45">
-        <v>0</v>
-      </c>
-      <c r="AI24" s="45">
-        <v>0</v>
-      </c>
-      <c r="AJ24" s="45">
-        <v>0</v>
-      </c>
-      <c r="AK24" s="45">
-        <v>0</v>
-      </c>
-      <c r="AL24" s="45">
-        <v>0</v>
-      </c>
-      <c r="AM24" s="45">
+      <c r="AB24" s="40">
+        <v>0</v>
+      </c>
+      <c r="AC24" s="40">
+        <v>0</v>
+      </c>
+      <c r="AD24" s="40">
+        <v>0</v>
+      </c>
+      <c r="AE24" s="40">
+        <v>0</v>
+      </c>
+      <c r="AF24" s="40">
+        <v>0</v>
+      </c>
+      <c r="AG24" s="40">
+        <v>0</v>
+      </c>
+      <c r="AH24" s="40">
+        <v>0</v>
+      </c>
+      <c r="AI24" s="40">
+        <v>0</v>
+      </c>
+      <c r="AJ24" s="40">
+        <v>0</v>
+      </c>
+      <c r="AK24" s="40">
+        <v>0</v>
+      </c>
+      <c r="AL24" s="40">
+        <v>0</v>
+      </c>
+      <c r="AM24" s="40">
         <v>7.7525000000000004</v>
       </c>
-      <c r="AN24" s="45">
+      <c r="AN24" s="40">
         <v>17.4922</v>
       </c>
-      <c r="AO24" s="45">
+      <c r="AO24" s="40">
         <v>20.453900000000001</v>
       </c>
-      <c r="AP24" s="45">
+      <c r="AP24" s="40">
         <v>22.773800000000001</v>
       </c>
-      <c r="AQ24" s="45">
+      <c r="AQ24" s="40">
         <v>23.786100000000001</v>
       </c>
-      <c r="AR24" s="45">
+      <c r="AR24" s="40">
         <v>24.974699999999999</v>
       </c>
-      <c r="AS24" s="45">
+      <c r="AS24" s="40">
         <v>24.350899999999999</v>
       </c>
-      <c r="AT24" s="45">
+      <c r="AT24" s="40">
         <v>29.445900000000002</v>
       </c>
-      <c r="AU24" s="45">
+      <c r="AU24" s="40">
         <v>31.3566</v>
       </c>
-      <c r="AV24" s="45">
+      <c r="AV24" s="40">
         <v>26.920400000000001</v>
       </c>
-      <c r="AW24" s="45">
+      <c r="AW24" s="40">
         <v>29.0212</v>
       </c>
-      <c r="AX24" s="45">
+      <c r="AX24" s="40">
         <v>28.322500000000002</v>
       </c>
     </row>
     <row r="25" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A25" s="43">
+      <c r="A25" s="38">
         <v>4</v>
       </c>
-      <c r="B25" s="44" t="s">
+      <c r="B25" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="C25" s="45">
+      <c r="C25" s="40">
         <v>1.5586</v>
       </c>
-      <c r="D25" s="45">
+      <c r="D25" s="40">
         <v>1.5488</v>
       </c>
-      <c r="E25" s="45">
+      <c r="E25" s="40">
         <v>1.5414000000000001</v>
       </c>
-      <c r="F25" s="45">
+      <c r="F25" s="40">
         <v>3.1949999999999998</v>
       </c>
-      <c r="G25" s="45">
+      <c r="G25" s="40">
         <v>2.9529000000000001</v>
       </c>
-      <c r="H25" s="45">
+      <c r="H25" s="40">
         <v>2.1137999999999999</v>
       </c>
-      <c r="I25" s="45">
+      <c r="I25" s="40">
         <v>3.9763000000000002</v>
       </c>
-      <c r="J25" s="45">
+      <c r="J25" s="40">
         <v>9.8012999999999995</v>
       </c>
-      <c r="K25" s="45">
+      <c r="K25" s="40">
         <v>13.5871</v>
       </c>
-      <c r="L25" s="45">
+      <c r="L25" s="40">
         <v>13.8225</v>
       </c>
-      <c r="M25" s="45">
+      <c r="M25" s="40">
         <v>6.8529</v>
       </c>
-      <c r="N25" s="45">
+      <c r="N25" s="40">
         <v>75.618799999999993</v>
       </c>
-      <c r="O25" s="45">
+      <c r="O25" s="40">
         <v>35.4343</v>
       </c>
-      <c r="P25" s="45">
+      <c r="P25" s="40">
         <v>13.2988</v>
       </c>
-      <c r="Q25" s="45">
+      <c r="Q25" s="40">
         <v>20.038799999999998</v>
       </c>
-      <c r="R25" s="45">
+      <c r="R25" s="40">
         <v>41.256300000000003</v>
       </c>
-      <c r="S25" s="45">
+      <c r="S25" s="40">
         <v>31.737100000000002</v>
       </c>
-      <c r="T25" s="45">
+      <c r="T25" s="40">
         <v>25.15</v>
       </c>
-      <c r="U25" s="45">
+      <c r="U25" s="40">
         <v>130.7938</v>
       </c>
-      <c r="V25" s="45">
+      <c r="V25" s="40">
         <v>67.722499999999997</v>
       </c>
-      <c r="W25" s="45">
+      <c r="W25" s="40">
         <v>51.3643</v>
       </c>
-      <c r="X25" s="45">
+      <c r="X25" s="40">
         <v>80.007499999999993</v>
       </c>
-      <c r="Y25" s="45">
+      <c r="Y25" s="40">
         <v>85.581400000000002</v>
       </c>
-      <c r="Z25" s="45">
+      <c r="Z25" s="40">
         <v>42.351300000000002</v>
       </c>
-      <c r="AA25" s="45">
+      <c r="AA25" s="40">
         <v>33.397100000000002</v>
       </c>
-      <c r="AB25" s="45">
+      <c r="AB25" s="40">
         <v>25.975000000000001</v>
       </c>
-      <c r="AC25" s="45">
+      <c r="AC25" s="40">
         <v>25.9513</v>
       </c>
-      <c r="AD25" s="45">
+      <c r="AD25" s="40">
         <v>31.504999999999999</v>
       </c>
-      <c r="AE25" s="45">
+      <c r="AE25" s="40">
         <v>30.1129</v>
       </c>
-      <c r="AF25" s="45">
+      <c r="AF25" s="40">
         <v>31.4588</v>
       </c>
-      <c r="AG25" s="45">
+      <c r="AG25" s="40">
         <v>35.185699999999997</v>
       </c>
-      <c r="AH25" s="45">
+      <c r="AH25" s="40">
         <v>35.352499999999999</v>
       </c>
-      <c r="AI25" s="45">
+      <c r="AI25" s="40">
         <v>30.222899999999999</v>
       </c>
-      <c r="AJ25" s="45">
+      <c r="AJ25" s="40">
         <v>26.004999999999999</v>
       </c>
-      <c r="AK25" s="45">
+      <c r="AK25" s="40">
         <v>21.0075</v>
       </c>
-      <c r="AL25" s="45">
+      <c r="AL25" s="40">
         <v>17.5288</v>
       </c>
-      <c r="AM25" s="45">
+      <c r="AM25" s="40">
         <v>14.154299999999999</v>
       </c>
-      <c r="AN25" s="45">
+      <c r="AN25" s="40">
         <v>13.016299999999999</v>
       </c>
-      <c r="AO25" s="45">
+      <c r="AO25" s="40">
         <v>11.946300000000001</v>
       </c>
-      <c r="AP25" s="45">
+      <c r="AP25" s="40">
         <v>10.3688</v>
       </c>
-      <c r="AQ25" s="45">
+      <c r="AQ25" s="40">
         <v>9.1670999999999996</v>
       </c>
-      <c r="AR25" s="45">
+      <c r="AR25" s="40">
         <v>8.6670999999999996</v>
       </c>
-      <c r="AS25" s="45">
+      <c r="AS25" s="40">
         <v>7.7385999999999999</v>
       </c>
-      <c r="AT25" s="45">
+      <c r="AT25" s="40">
         <v>7.1688000000000001</v>
       </c>
-      <c r="AU25" s="45">
+      <c r="AU25" s="40">
         <v>6.4470999999999998</v>
       </c>
-      <c r="AV25" s="45">
+      <c r="AV25" s="40">
         <v>5.8550000000000004</v>
       </c>
-      <c r="AW25" s="45">
+      <c r="AW25" s="40">
         <v>6.1375000000000002</v>
       </c>
-      <c r="AX25" s="45">
+      <c r="AX25" s="40">
         <v>5.4462999999999999</v>
       </c>
     </row>
     <row r="26" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A26" s="43">
+      <c r="A26" s="38">
         <v>4</v>
       </c>
-      <c r="B26" s="44" t="s">
+      <c r="B26" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="45">
-        <v>0</v>
-      </c>
-      <c r="D26" s="45">
+      <c r="C26" s="40">
+        <v>0</v>
+      </c>
+      <c r="D26" s="40">
         <v>0.41439999999999999</v>
       </c>
-      <c r="E26" s="45">
-        <v>0</v>
-      </c>
-      <c r="F26" s="45">
+      <c r="E26" s="40">
+        <v>0</v>
+      </c>
+      <c r="F26" s="40">
         <v>4.2305000000000001</v>
       </c>
-      <c r="G26" s="45">
+      <c r="G26" s="40">
         <v>22.868300000000001</v>
       </c>
-      <c r="H26" s="45">
+      <c r="H26" s="40">
         <v>11.2712</v>
       </c>
-      <c r="I26" s="45">
+      <c r="I26" s="40">
         <v>14.9282</v>
       </c>
-      <c r="J26" s="45">
+      <c r="J26" s="40">
         <v>42.6873</v>
       </c>
-      <c r="K26" s="45">
+      <c r="K26" s="40">
         <v>60.828899999999997</v>
       </c>
-      <c r="L26" s="45">
+      <c r="L26" s="40">
         <v>84.741100000000003</v>
       </c>
-      <c r="M26" s="45">
+      <c r="M26" s="40">
         <v>20.628799999999998</v>
       </c>
-      <c r="N26" s="45">
+      <c r="N26" s="40">
         <v>313.75189999999998</v>
       </c>
-      <c r="O26" s="45">
+      <c r="O26" s="40">
         <v>129.73660000000001</v>
       </c>
-      <c r="P26" s="45">
+      <c r="P26" s="40">
         <v>103.4714</v>
       </c>
-      <c r="Q26" s="45">
+      <c r="Q26" s="40">
         <v>96.967500000000001</v>
       </c>
-      <c r="R26" s="45">
+      <c r="R26" s="40">
         <v>94.388800000000003</v>
       </c>
-      <c r="S26" s="45">
+      <c r="S26" s="40">
         <v>66.02</v>
       </c>
-      <c r="T26" s="45">
+      <c r="T26" s="40">
         <v>53.8825</v>
       </c>
-      <c r="U26" s="45">
+      <c r="U26" s="40">
         <v>103.8313</v>
       </c>
-      <c r="V26" s="45">
+      <c r="V26" s="40">
         <v>147.11500000000001</v>
       </c>
-      <c r="W26" s="45">
+      <c r="W26" s="40">
         <v>129.2629</v>
       </c>
-      <c r="X26" s="45">
+      <c r="X26" s="40">
         <v>126.9688</v>
       </c>
-      <c r="Y26" s="45">
+      <c r="Y26" s="40">
         <v>125.6914</v>
       </c>
-      <c r="Z26" s="45">
+      <c r="Z26" s="40">
         <v>104.75749999999999</v>
       </c>
-      <c r="AA26" s="45">
+      <c r="AA26" s="40">
         <v>68.404300000000006</v>
       </c>
-      <c r="AB26" s="45">
+      <c r="AB26" s="40">
         <v>38.643799999999999</v>
       </c>
-      <c r="AC26" s="45">
+      <c r="AC26" s="40">
         <v>20.801300000000001</v>
       </c>
-      <c r="AD26" s="45">
+      <c r="AD26" s="40">
         <v>26.664999999999999</v>
       </c>
-      <c r="AE26" s="45">
+      <c r="AE26" s="40">
         <v>10.6557</v>
       </c>
-      <c r="AF26" s="45">
+      <c r="AF26" s="40">
         <v>13.8263</v>
       </c>
-      <c r="AG26" s="45">
+      <c r="AG26" s="40">
         <v>35.278599999999997</v>
       </c>
-      <c r="AH26" s="45">
+      <c r="AH26" s="40">
         <v>1.61E-2</v>
       </c>
-      <c r="AI26" s="45">
+      <c r="AI26" s="40">
         <v>1.61E-2</v>
       </c>
-      <c r="AJ26" s="45">
+      <c r="AJ26" s="40">
         <v>1.61E-2</v>
       </c>
-      <c r="AK26" s="45">
+      <c r="AK26" s="40">
         <v>1.61E-2</v>
       </c>
-      <c r="AL26" s="45">
+      <c r="AL26" s="40">
         <v>1.61E-2</v>
       </c>
-      <c r="AM26" s="45">
+      <c r="AM26" s="40">
         <v>1.61E-2</v>
       </c>
-      <c r="AN26" s="45">
+      <c r="AN26" s="40">
         <v>1.61E-2</v>
       </c>
-      <c r="AO26" s="45">
+      <c r="AO26" s="40">
         <v>1.61E-2</v>
       </c>
-      <c r="AP26" s="45">
+      <c r="AP26" s="40">
         <v>1.0161</v>
       </c>
-      <c r="AQ26" s="45">
+      <c r="AQ26" s="40">
         <v>2.0160999999999998</v>
       </c>
-      <c r="AR26" s="45">
+      <c r="AR26" s="40">
         <v>3.0160999999999998</v>
       </c>
-      <c r="AS26" s="45">
+      <c r="AS26" s="40">
         <v>4.0160999999999998</v>
       </c>
-      <c r="AT26" s="45">
-        <v>0</v>
-      </c>
-      <c r="AU26" s="45">
-        <v>0</v>
-      </c>
-      <c r="AV26" s="45">
-        <v>0</v>
-      </c>
-      <c r="AW26" s="45">
-        <v>0</v>
-      </c>
-      <c r="AX26" s="45">
+      <c r="AT26" s="40">
+        <v>0</v>
+      </c>
+      <c r="AU26" s="40">
+        <v>0</v>
+      </c>
+      <c r="AV26" s="40">
+        <v>0</v>
+      </c>
+      <c r="AW26" s="40">
+        <v>0</v>
+      </c>
+      <c r="AX26" s="40">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A27" s="41">
+      <c r="A27" s="36">
         <v>5</v>
       </c>
-      <c r="B27" s="42" t="s">
+      <c r="B27" s="37" t="s">
         <v>2</v>
       </c>
       <c r="C27" s="34">
@@ -9585,762 +9616,762 @@
       </c>
     </row>
     <row r="28" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A28" s="43">
+      <c r="A28" s="38">
         <v>5</v>
       </c>
-      <c r="B28" s="44" t="s">
+      <c r="B28" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="C28" s="45">
+      <c r="C28" s="40">
         <v>0.30380000000000001</v>
       </c>
-      <c r="D28" s="45">
+      <c r="D28" s="40">
         <v>0.33550000000000002</v>
       </c>
-      <c r="E28" s="45">
+      <c r="E28" s="40">
         <v>0.33329999999999999</v>
       </c>
-      <c r="F28" s="45">
+      <c r="F28" s="40">
         <v>0.57740000000000002</v>
       </c>
-      <c r="G28" s="45">
+      <c r="G28" s="40">
         <v>1.2271000000000001</v>
       </c>
-      <c r="H28" s="45">
+      <c r="H28" s="40">
         <v>0.99550000000000005</v>
       </c>
-      <c r="I28" s="45">
+      <c r="I28" s="40">
         <v>1.2551000000000001</v>
       </c>
-      <c r="J28" s="45">
+      <c r="J28" s="40">
         <v>3.5543999999999998</v>
       </c>
-      <c r="K28" s="45">
+      <c r="K28" s="40">
         <v>6.2462</v>
       </c>
-      <c r="L28" s="45">
+      <c r="L28" s="40">
         <v>8.4306999999999999</v>
       </c>
-      <c r="M28" s="45">
+      <c r="M28" s="40">
         <v>3.9758</v>
       </c>
-      <c r="N28" s="45">
+      <c r="N28" s="40">
         <v>46.954700000000003</v>
       </c>
-      <c r="O28" s="45">
+      <c r="O28" s="40">
         <v>15.176</v>
       </c>
-      <c r="P28" s="45">
+      <c r="P28" s="40">
         <v>10.0284</v>
       </c>
-      <c r="Q28" s="45">
+      <c r="Q28" s="40">
         <v>9.2880000000000003</v>
       </c>
-      <c r="R28" s="45">
+      <c r="R28" s="40">
         <v>9.8729999999999993</v>
       </c>
-      <c r="S28" s="45">
+      <c r="S28" s="40">
         <v>8.5383999999999993</v>
       </c>
-      <c r="T28" s="45">
+      <c r="T28" s="40">
         <v>7.0475000000000003</v>
       </c>
-      <c r="U28" s="45">
+      <c r="U28" s="40">
         <v>28.213899999999999</v>
       </c>
-      <c r="V28" s="45">
+      <c r="V28" s="40">
         <v>16.5334</v>
       </c>
-      <c r="W28" s="45">
+      <c r="W28" s="40">
         <v>9.8302999999999994</v>
       </c>
-      <c r="X28" s="45">
+      <c r="X28" s="40">
         <v>9.7766999999999999</v>
       </c>
-      <c r="Y28" s="45">
+      <c r="Y28" s="40">
         <v>9.7760999999999996</v>
       </c>
-      <c r="Z28" s="45">
+      <c r="Z28" s="40">
         <v>5.6445999999999996</v>
       </c>
-      <c r="AA28" s="45">
+      <c r="AA28" s="40">
         <v>4.9169999999999998</v>
       </c>
-      <c r="AB28" s="45">
+      <c r="AB28" s="40">
         <v>4.3285</v>
       </c>
-      <c r="AC28" s="45">
+      <c r="AC28" s="40">
         <v>6.1745000000000001</v>
       </c>
-      <c r="AD28" s="45">
+      <c r="AD28" s="40">
         <v>7.7904999999999998</v>
       </c>
-      <c r="AE28" s="45">
+      <c r="AE28" s="40">
         <v>6.7957000000000001</v>
       </c>
-      <c r="AF28" s="45">
+      <c r="AF28" s="40">
         <v>7.8418999999999999</v>
       </c>
-      <c r="AG28" s="45">
+      <c r="AG28" s="40">
         <v>8.4492999999999991</v>
       </c>
-      <c r="AH28" s="45">
+      <c r="AH28" s="40">
         <v>9.7650000000000006</v>
       </c>
-      <c r="AI28" s="45">
+      <c r="AI28" s="40">
         <v>6.3874000000000004</v>
       </c>
-      <c r="AJ28" s="45">
+      <c r="AJ28" s="40">
         <v>5.8741000000000003</v>
       </c>
-      <c r="AK28" s="45">
+      <c r="AK28" s="40">
         <v>4.6536999999999997</v>
       </c>
-      <c r="AL28" s="45">
+      <c r="AL28" s="40">
         <v>4.0388999999999999</v>
       </c>
-      <c r="AM28" s="45">
+      <c r="AM28" s="40">
         <v>2.8151000000000002</v>
       </c>
-      <c r="AN28" s="45">
+      <c r="AN28" s="40">
         <v>3.7141000000000002</v>
       </c>
-      <c r="AO28" s="45">
+      <c r="AO28" s="40">
         <v>4.0777000000000001</v>
       </c>
-      <c r="AP28" s="45">
+      <c r="AP28" s="40">
         <v>4.4039999999999999</v>
       </c>
-      <c r="AQ28" s="45">
+      <c r="AQ28" s="40">
         <v>3.7584</v>
       </c>
-      <c r="AR28" s="45">
+      <c r="AR28" s="40">
         <v>4.1703999999999999</v>
       </c>
-      <c r="AS28" s="45">
+      <c r="AS28" s="40">
         <v>3.5545</v>
       </c>
-      <c r="AT28" s="45">
+      <c r="AT28" s="40">
         <v>3.5249999999999999</v>
       </c>
-      <c r="AU28" s="45">
+      <c r="AU28" s="40">
         <v>2.6757</v>
       </c>
-      <c r="AV28" s="45">
+      <c r="AV28" s="40">
         <v>2.6162999999999998</v>
       </c>
-      <c r="AW28" s="45">
+      <c r="AW28" s="40">
         <v>1.7538</v>
       </c>
-      <c r="AX28" s="45">
+      <c r="AX28" s="40">
         <v>1.9450000000000001</v>
       </c>
     </row>
     <row r="29" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A29" s="43">
+      <c r="A29" s="38">
         <v>5</v>
       </c>
-      <c r="B29" s="44" t="s">
+      <c r="B29" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="C29" s="45">
+      <c r="C29" s="40">
         <v>7.9802999999999997</v>
       </c>
-      <c r="D29" s="45">
+      <c r="D29" s="40">
         <v>7.6040999999999999</v>
       </c>
-      <c r="E29" s="45">
+      <c r="E29" s="40">
         <v>7.5530999999999997</v>
       </c>
-      <c r="F29" s="45">
+      <c r="F29" s="40">
         <v>13.176500000000001</v>
       </c>
-      <c r="G29" s="45">
+      <c r="G29" s="40">
         <v>12.1896</v>
       </c>
-      <c r="H29" s="45">
+      <c r="H29" s="40">
         <v>9.8892000000000007</v>
       </c>
-      <c r="I29" s="45">
+      <c r="I29" s="40">
         <v>12.4674</v>
       </c>
-      <c r="J29" s="45">
+      <c r="J29" s="40">
         <v>35.308199999999999</v>
       </c>
-      <c r="K29" s="45">
+      <c r="K29" s="40">
         <v>62.047699999999999</v>
       </c>
-      <c r="L29" s="45">
+      <c r="L29" s="40">
         <v>83.747799999999998</v>
       </c>
-      <c r="M29" s="45">
+      <c r="M29" s="40">
         <v>39.494199999999999</v>
       </c>
-      <c r="N29" s="45">
+      <c r="N29" s="40">
         <v>466.43060000000003</v>
       </c>
-      <c r="O29" s="45">
+      <c r="O29" s="40">
         <v>150.7527</v>
       </c>
-      <c r="P29" s="45">
+      <c r="P29" s="40">
         <v>99.618600000000001</v>
       </c>
-      <c r="Q29" s="45">
+      <c r="Q29" s="40">
         <v>92.263400000000004</v>
       </c>
-      <c r="R29" s="45">
+      <c r="R29" s="40">
         <v>98.0745</v>
       </c>
-      <c r="S29" s="45">
+      <c r="S29" s="40">
         <v>84.816999999999993</v>
       </c>
-      <c r="T29" s="45">
+      <c r="T29" s="40">
         <v>70.007300000000001</v>
       </c>
-      <c r="U29" s="45">
+      <c r="U29" s="40">
         <v>280.26679999999999</v>
       </c>
-      <c r="V29" s="45">
+      <c r="V29" s="40">
         <v>164.23670000000001</v>
       </c>
-      <c r="W29" s="45">
+      <c r="W29" s="40">
         <v>131.8903</v>
       </c>
-      <c r="X29" s="45">
+      <c r="X29" s="40">
         <v>186.15350000000001</v>
       </c>
-      <c r="Y29" s="45">
+      <c r="Y29" s="40">
         <v>186.14359999999999</v>
       </c>
-      <c r="Z29" s="45">
+      <c r="Z29" s="40">
         <v>112.143</v>
       </c>
-      <c r="AA29" s="45">
+      <c r="AA29" s="40">
         <v>95.753799999999998</v>
       </c>
-      <c r="AB29" s="45">
+      <c r="AB29" s="40">
         <v>84.281400000000005</v>
       </c>
-      <c r="AC29" s="45">
+      <c r="AC29" s="40">
         <v>90.786000000000001</v>
       </c>
-      <c r="AD29" s="45">
+      <c r="AD29" s="40">
         <v>104.1803</v>
       </c>
-      <c r="AE29" s="45">
+      <c r="AE29" s="40">
         <v>102.56100000000001</v>
       </c>
-      <c r="AF29" s="45">
+      <c r="AF29" s="40">
         <v>105.1374</v>
       </c>
-      <c r="AG29" s="45">
+      <c r="AG29" s="40">
         <v>115.3991</v>
       </c>
-      <c r="AH29" s="45">
+      <c r="AH29" s="40">
         <v>133.2433</v>
       </c>
-      <c r="AI29" s="45">
+      <c r="AI29" s="40">
         <v>112.6189</v>
       </c>
-      <c r="AJ29" s="45">
+      <c r="AJ29" s="40">
         <v>94.846800000000002</v>
       </c>
-      <c r="AK29" s="45">
+      <c r="AK29" s="40">
         <v>74.649699999999996</v>
       </c>
-      <c r="AL29" s="45">
+      <c r="AL29" s="40">
         <v>63.080500000000001</v>
       </c>
-      <c r="AM29" s="45">
+      <c r="AM29" s="40">
         <v>49.628599999999999</v>
       </c>
-      <c r="AN29" s="45">
+      <c r="AN29" s="40">
         <v>42.404299999999999</v>
       </c>
-      <c r="AO29" s="45">
+      <c r="AO29" s="40">
         <v>37.862099999999998</v>
       </c>
-      <c r="AP29" s="45">
+      <c r="AP29" s="40">
         <v>32.775399999999998</v>
       </c>
-      <c r="AQ29" s="45">
+      <c r="AQ29" s="40">
         <v>29.386700000000001</v>
       </c>
-      <c r="AR29" s="45">
+      <c r="AR29" s="40">
         <v>27.220500000000001</v>
       </c>
-      <c r="AS29" s="45">
+      <c r="AS29" s="40">
         <v>25.061699999999998</v>
       </c>
-      <c r="AT29" s="45">
+      <c r="AT29" s="40">
         <v>22.666399999999999</v>
       </c>
-      <c r="AU29" s="45">
+      <c r="AU29" s="40">
         <v>19.9833</v>
       </c>
-      <c r="AV29" s="45">
+      <c r="AV29" s="40">
         <v>18.886299999999999</v>
       </c>
-      <c r="AW29" s="45">
+      <c r="AW29" s="40">
         <v>19.750699999999998</v>
       </c>
-      <c r="AX29" s="45">
+      <c r="AX29" s="40">
         <v>18.032399999999999</v>
       </c>
     </row>
     <row r="30" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A30" s="43">
+      <c r="A30" s="38">
         <v>5</v>
       </c>
-      <c r="B30" s="44" t="s">
+      <c r="B30" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="C30" s="45">
+      <c r="C30" s="40">
         <v>24.087800000000001</v>
       </c>
-      <c r="D30" s="45">
+      <c r="D30" s="40">
         <v>24.008700000000001</v>
       </c>
-      <c r="E30" s="45">
+      <c r="E30" s="40">
         <v>19.410900000000002</v>
       </c>
-      <c r="F30" s="45">
+      <c r="F30" s="40">
         <v>20.5943</v>
       </c>
-      <c r="G30" s="45">
+      <c r="G30" s="40">
         <v>18.503900000000002</v>
       </c>
-      <c r="H30" s="45">
+      <c r="H30" s="40">
         <v>15.536300000000001</v>
       </c>
-      <c r="I30" s="45">
+      <c r="I30" s="40">
         <v>29.118099999999998</v>
       </c>
-      <c r="J30" s="45">
+      <c r="J30" s="40">
         <v>49.311399999999999</v>
       </c>
-      <c r="K30" s="45">
+      <c r="K30" s="40">
         <v>57.905799999999999</v>
       </c>
-      <c r="L30" s="45">
+      <c r="L30" s="40">
         <v>95.133099999999999</v>
       </c>
-      <c r="M30" s="45">
+      <c r="M30" s="40">
         <v>20.4483</v>
       </c>
-      <c r="N30" s="45">
+      <c r="N30" s="40">
         <v>311.5539</v>
       </c>
-      <c r="O30" s="45">
+      <c r="O30" s="40">
         <v>69.771000000000001</v>
       </c>
-      <c r="P30" s="45">
+      <c r="P30" s="40">
         <v>11.9916</v>
       </c>
-      <c r="Q30" s="45">
+      <c r="Q30" s="40">
         <v>29.9984</v>
       </c>
-      <c r="R30" s="45">
+      <c r="R30" s="40">
         <v>105.80710000000001</v>
       </c>
-      <c r="S30" s="45">
+      <c r="S30" s="40">
         <v>75.442899999999995</v>
       </c>
-      <c r="T30" s="45">
+      <c r="T30" s="40">
         <v>56.216500000000003</v>
       </c>
-      <c r="U30" s="45">
+      <c r="U30" s="40">
         <v>260.79180000000002</v>
       </c>
-      <c r="V30" s="45">
+      <c r="V30" s="40">
         <v>95.894900000000007</v>
       </c>
-      <c r="W30" s="45">
+      <c r="W30" s="40">
         <v>58.996899999999997</v>
       </c>
-      <c r="X30" s="45">
+      <c r="X30" s="40">
         <v>121.681</v>
       </c>
-      <c r="Y30" s="45">
+      <c r="Y30" s="40">
         <v>165.72890000000001</v>
       </c>
-      <c r="Z30" s="45">
+      <c r="Z30" s="40">
         <v>44.283200000000001</v>
       </c>
-      <c r="AA30" s="45">
+      <c r="AA30" s="40">
         <v>23.104800000000001</v>
       </c>
-      <c r="AB30" s="45">
-        <v>0</v>
-      </c>
-      <c r="AC30" s="45">
-        <v>0</v>
-      </c>
-      <c r="AD30" s="45">
-        <v>0</v>
-      </c>
-      <c r="AE30" s="45">
-        <v>0</v>
-      </c>
-      <c r="AF30" s="45">
-        <v>0</v>
-      </c>
-      <c r="AG30" s="45">
-        <v>0</v>
-      </c>
-      <c r="AH30" s="45">
-        <v>0</v>
-      </c>
-      <c r="AI30" s="45">
-        <v>0</v>
-      </c>
-      <c r="AJ30" s="45">
-        <v>0</v>
-      </c>
-      <c r="AK30" s="45">
-        <v>0</v>
-      </c>
-      <c r="AL30" s="45">
-        <v>0</v>
-      </c>
-      <c r="AM30" s="45">
+      <c r="AB30" s="40">
+        <v>0</v>
+      </c>
+      <c r="AC30" s="40">
+        <v>0</v>
+      </c>
+      <c r="AD30" s="40">
+        <v>0</v>
+      </c>
+      <c r="AE30" s="40">
+        <v>0</v>
+      </c>
+      <c r="AF30" s="40">
+        <v>0</v>
+      </c>
+      <c r="AG30" s="40">
+        <v>0</v>
+      </c>
+      <c r="AH30" s="40">
+        <v>0</v>
+      </c>
+      <c r="AI30" s="40">
+        <v>0</v>
+      </c>
+      <c r="AJ30" s="40">
+        <v>0</v>
+      </c>
+      <c r="AK30" s="40">
+        <v>0</v>
+      </c>
+      <c r="AL30" s="40">
+        <v>0</v>
+      </c>
+      <c r="AM30" s="40">
         <v>7.7525000000000004</v>
       </c>
-      <c r="AN30" s="45">
+      <c r="AN30" s="40">
         <v>17.4922</v>
       </c>
-      <c r="AO30" s="45">
+      <c r="AO30" s="40">
         <v>20.453900000000001</v>
       </c>
-      <c r="AP30" s="45">
+      <c r="AP30" s="40">
         <v>22.773800000000001</v>
       </c>
-      <c r="AQ30" s="45">
+      <c r="AQ30" s="40">
         <v>23.786100000000001</v>
       </c>
-      <c r="AR30" s="45">
+      <c r="AR30" s="40">
         <v>24.974699999999999</v>
       </c>
-      <c r="AS30" s="45">
+      <c r="AS30" s="40">
         <v>24.350899999999999</v>
       </c>
-      <c r="AT30" s="45">
+      <c r="AT30" s="40">
         <v>29.445900000000002</v>
       </c>
-      <c r="AU30" s="45">
+      <c r="AU30" s="40">
         <v>31.3566</v>
       </c>
-      <c r="AV30" s="45">
+      <c r="AV30" s="40">
         <v>26.920400000000001</v>
       </c>
-      <c r="AW30" s="45">
+      <c r="AW30" s="40">
         <v>29.0212</v>
       </c>
-      <c r="AX30" s="45">
+      <c r="AX30" s="40">
         <v>28.322500000000002</v>
       </c>
     </row>
     <row r="31" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A31" s="43">
+      <c r="A31" s="38">
         <v>5</v>
       </c>
-      <c r="B31" s="44" t="s">
+      <c r="B31" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="C31" s="45">
+      <c r="C31" s="40">
         <v>1.5586</v>
       </c>
-      <c r="D31" s="45">
+      <c r="D31" s="40">
         <v>1.5488</v>
       </c>
-      <c r="E31" s="45">
+      <c r="E31" s="40">
         <v>1.5414000000000001</v>
       </c>
-      <c r="F31" s="45">
+      <c r="F31" s="40">
         <v>3.1949999999999998</v>
       </c>
-      <c r="G31" s="45">
+      <c r="G31" s="40">
         <v>2.9529000000000001</v>
       </c>
-      <c r="H31" s="45">
+      <c r="H31" s="40">
         <v>2.1137999999999999</v>
       </c>
-      <c r="I31" s="45">
+      <c r="I31" s="40">
         <v>3.9763000000000002</v>
       </c>
-      <c r="J31" s="45">
+      <c r="J31" s="40">
         <v>9.8012999999999995</v>
       </c>
-      <c r="K31" s="45">
+      <c r="K31" s="40">
         <v>13.5871</v>
       </c>
-      <c r="L31" s="45">
+      <c r="L31" s="40">
         <v>13.8225</v>
       </c>
-      <c r="M31" s="45">
+      <c r="M31" s="40">
         <v>6.8529</v>
       </c>
-      <c r="N31" s="45">
+      <c r="N31" s="40">
         <v>75.618799999999993</v>
       </c>
-      <c r="O31" s="45">
+      <c r="O31" s="40">
         <v>35.4343</v>
       </c>
-      <c r="P31" s="45">
+      <c r="P31" s="40">
         <v>13.2988</v>
       </c>
-      <c r="Q31" s="45">
+      <c r="Q31" s="40">
         <v>20.038799999999998</v>
       </c>
-      <c r="R31" s="45">
+      <c r="R31" s="40">
         <v>41.256300000000003</v>
       </c>
-      <c r="S31" s="45">
+      <c r="S31" s="40">
         <v>31.737100000000002</v>
       </c>
-      <c r="T31" s="45">
+      <c r="T31" s="40">
         <v>25.15</v>
       </c>
-      <c r="U31" s="45">
+      <c r="U31" s="40">
         <v>130.7938</v>
       </c>
-      <c r="V31" s="45">
+      <c r="V31" s="40">
         <v>67.722499999999997</v>
       </c>
-      <c r="W31" s="45">
+      <c r="W31" s="40">
         <v>51.3643</v>
       </c>
-      <c r="X31" s="45">
+      <c r="X31" s="40">
         <v>80.007499999999993</v>
       </c>
-      <c r="Y31" s="45">
+      <c r="Y31" s="40">
         <v>85.581400000000002</v>
       </c>
-      <c r="Z31" s="45">
+      <c r="Z31" s="40">
         <v>42.351300000000002</v>
       </c>
-      <c r="AA31" s="45">
+      <c r="AA31" s="40">
         <v>33.397100000000002</v>
       </c>
-      <c r="AB31" s="45">
+      <c r="AB31" s="40">
         <v>25.975000000000001</v>
       </c>
-      <c r="AC31" s="45">
+      <c r="AC31" s="40">
         <v>25.9513</v>
       </c>
-      <c r="AD31" s="45">
+      <c r="AD31" s="40">
         <v>31.504999999999999</v>
       </c>
-      <c r="AE31" s="45">
+      <c r="AE31" s="40">
         <v>30.1129</v>
       </c>
-      <c r="AF31" s="45">
+      <c r="AF31" s="40">
         <v>31.4588</v>
       </c>
-      <c r="AG31" s="45">
+      <c r="AG31" s="40">
         <v>35.185699999999997</v>
       </c>
-      <c r="AH31" s="45">
+      <c r="AH31" s="40">
         <v>35.352499999999999</v>
       </c>
-      <c r="AI31" s="45">
+      <c r="AI31" s="40">
         <v>30.222899999999999</v>
       </c>
-      <c r="AJ31" s="45">
+      <c r="AJ31" s="40">
         <v>26.004999999999999</v>
       </c>
-      <c r="AK31" s="45">
+      <c r="AK31" s="40">
         <v>21.0075</v>
       </c>
-      <c r="AL31" s="45">
+      <c r="AL31" s="40">
         <v>17.5288</v>
       </c>
-      <c r="AM31" s="45">
+      <c r="AM31" s="40">
         <v>14.154299999999999</v>
       </c>
-      <c r="AN31" s="45">
+      <c r="AN31" s="40">
         <v>13.016299999999999</v>
       </c>
-      <c r="AO31" s="45">
+      <c r="AO31" s="40">
         <v>11.946300000000001</v>
       </c>
-      <c r="AP31" s="45">
+      <c r="AP31" s="40">
         <v>10.3688</v>
       </c>
-      <c r="AQ31" s="45">
+      <c r="AQ31" s="40">
         <v>9.1670999999999996</v>
       </c>
-      <c r="AR31" s="45">
+      <c r="AR31" s="40">
         <v>8.6670999999999996</v>
       </c>
-      <c r="AS31" s="45">
+      <c r="AS31" s="40">
         <v>7.7385999999999999</v>
       </c>
-      <c r="AT31" s="45">
+      <c r="AT31" s="40">
         <v>7.1688000000000001</v>
       </c>
-      <c r="AU31" s="45">
+      <c r="AU31" s="40">
         <v>6.4470999999999998</v>
       </c>
-      <c r="AV31" s="45">
+      <c r="AV31" s="40">
         <v>5.8550000000000004</v>
       </c>
-      <c r="AW31" s="45">
+      <c r="AW31" s="40">
         <v>6.1375000000000002</v>
       </c>
-      <c r="AX31" s="45">
+      <c r="AX31" s="40">
         <v>5.4462999999999999</v>
       </c>
     </row>
     <row r="32" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A32" s="43">
+      <c r="A32" s="38">
         <v>5</v>
       </c>
-      <c r="B32" s="44" t="s">
+      <c r="B32" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="C32" s="45">
-        <v>0</v>
-      </c>
-      <c r="D32" s="45">
+      <c r="C32" s="40">
+        <v>0</v>
+      </c>
+      <c r="D32" s="40">
         <v>0.41439999999999999</v>
       </c>
-      <c r="E32" s="45">
-        <v>0</v>
-      </c>
-      <c r="F32" s="45">
+      <c r="E32" s="40">
+        <v>0</v>
+      </c>
+      <c r="F32" s="40">
         <v>4.2305000000000001</v>
       </c>
-      <c r="G32" s="45">
+      <c r="G32" s="40">
         <v>22.868300000000001</v>
       </c>
-      <c r="H32" s="45">
+      <c r="H32" s="40">
         <v>11.2712</v>
       </c>
-      <c r="I32" s="45">
+      <c r="I32" s="40">
         <v>14.9282</v>
       </c>
-      <c r="J32" s="45">
+      <c r="J32" s="40">
         <v>42.6873</v>
       </c>
-      <c r="K32" s="45">
+      <c r="K32" s="40">
         <v>60.828899999999997</v>
       </c>
-      <c r="L32" s="45">
+      <c r="L32" s="40">
         <v>84.741100000000003</v>
       </c>
-      <c r="M32" s="45">
+      <c r="M32" s="40">
         <v>20.628799999999998</v>
       </c>
-      <c r="N32" s="45">
+      <c r="N32" s="40">
         <v>313.75189999999998</v>
       </c>
-      <c r="O32" s="45">
+      <c r="O32" s="40">
         <v>129.73660000000001</v>
       </c>
-      <c r="P32" s="45">
+      <c r="P32" s="40">
         <v>103.4714</v>
       </c>
-      <c r="Q32" s="45">
+      <c r="Q32" s="40">
         <v>96.967500000000001</v>
       </c>
-      <c r="R32" s="45">
+      <c r="R32" s="40">
         <v>94.388800000000003</v>
       </c>
-      <c r="S32" s="45">
+      <c r="S32" s="40">
         <v>66.02</v>
       </c>
-      <c r="T32" s="45">
+      <c r="T32" s="40">
         <v>53.8825</v>
       </c>
-      <c r="U32" s="45">
+      <c r="U32" s="40">
         <v>103.8313</v>
       </c>
-      <c r="V32" s="45">
+      <c r="V32" s="40">
         <v>147.11500000000001</v>
       </c>
-      <c r="W32" s="45">
+      <c r="W32" s="40">
         <v>129.2629</v>
       </c>
-      <c r="X32" s="45">
+      <c r="X32" s="40">
         <v>126.9688</v>
       </c>
-      <c r="Y32" s="45">
+      <c r="Y32" s="40">
         <v>125.6914</v>
       </c>
-      <c r="Z32" s="45">
+      <c r="Z32" s="40">
         <v>104.75749999999999</v>
       </c>
-      <c r="AA32" s="45">
+      <c r="AA32" s="40">
         <v>68.404300000000006</v>
       </c>
-      <c r="AB32" s="45">
+      <c r="AB32" s="40">
         <v>38.643799999999999</v>
       </c>
-      <c r="AC32" s="45">
+      <c r="AC32" s="40">
         <v>20.801300000000001</v>
       </c>
-      <c r="AD32" s="45">
+      <c r="AD32" s="40">
         <v>26.664999999999999</v>
       </c>
-      <c r="AE32" s="45">
+      <c r="AE32" s="40">
         <v>10.6557</v>
       </c>
-      <c r="AF32" s="45">
+      <c r="AF32" s="40">
         <v>13.8263</v>
       </c>
-      <c r="AG32" s="45">
+      <c r="AG32" s="40">
         <v>35.278599999999997</v>
       </c>
-      <c r="AH32" s="45">
+      <c r="AH32" s="40">
         <v>1.61E-2</v>
       </c>
-      <c r="AI32" s="45">
+      <c r="AI32" s="40">
         <v>1.61E-2</v>
       </c>
-      <c r="AJ32" s="45">
+      <c r="AJ32" s="40">
         <v>1.61E-2</v>
       </c>
-      <c r="AK32" s="45">
+      <c r="AK32" s="40">
         <v>1.61E-2</v>
       </c>
-      <c r="AL32" s="45">
+      <c r="AL32" s="40">
         <v>1.61E-2</v>
       </c>
-      <c r="AM32" s="45">
+      <c r="AM32" s="40">
         <v>1.61E-2</v>
       </c>
-      <c r="AN32" s="45">
+      <c r="AN32" s="40">
         <v>1.61E-2</v>
       </c>
-      <c r="AO32" s="45">
+      <c r="AO32" s="40">
         <v>1.61E-2</v>
       </c>
-      <c r="AP32" s="45">
+      <c r="AP32" s="40">
         <v>1.0161</v>
       </c>
-      <c r="AQ32" s="45">
+      <c r="AQ32" s="40">
         <v>2.0160999999999998</v>
       </c>
-      <c r="AR32" s="45">
+      <c r="AR32" s="40">
         <v>3.0160999999999998</v>
       </c>
-      <c r="AS32" s="45">
+      <c r="AS32" s="40">
         <v>4.0160999999999998</v>
       </c>
-      <c r="AT32" s="45">
-        <v>0</v>
-      </c>
-      <c r="AU32" s="45">
-        <v>0</v>
-      </c>
-      <c r="AV32" s="45">
-        <v>0</v>
-      </c>
-      <c r="AW32" s="45">
-        <v>0</v>
-      </c>
-      <c r="AX32" s="45">
+      <c r="AT32" s="40">
+        <v>0</v>
+      </c>
+      <c r="AU32" s="40">
+        <v>0</v>
+      </c>
+      <c r="AV32" s="40">
+        <v>0</v>
+      </c>
+      <c r="AW32" s="40">
+        <v>0</v>
+      </c>
+      <c r="AX32" s="40">
         <v>0</v>
       </c>
     </row>
@@ -10372,154 +10403,154 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="42" t="s">
         <v>85</v>
       </c>
-      <c r="C1" s="48">
+      <c r="C1" s="43">
         <v>1</v>
       </c>
-      <c r="D1" s="48">
+      <c r="D1" s="43">
         <v>2</v>
       </c>
-      <c r="E1" s="48">
+      <c r="E1" s="43">
         <v>3</v>
       </c>
-      <c r="F1" s="48">
+      <c r="F1" s="43">
         <v>4</v>
       </c>
-      <c r="G1" s="48">
+      <c r="G1" s="43">
         <v>5</v>
       </c>
-      <c r="H1" s="48">
+      <c r="H1" s="43">
         <v>6</v>
       </c>
-      <c r="I1" s="48">
+      <c r="I1" s="43">
         <v>7</v>
       </c>
-      <c r="J1" s="48">
+      <c r="J1" s="43">
         <v>8</v>
       </c>
-      <c r="K1" s="48">
+      <c r="K1" s="43">
         <v>9</v>
       </c>
-      <c r="L1" s="48">
+      <c r="L1" s="43">
         <v>10</v>
       </c>
-      <c r="M1" s="48">
+      <c r="M1" s="43">
         <v>11</v>
       </c>
-      <c r="N1" s="48">
+      <c r="N1" s="43">
         <v>12</v>
       </c>
-      <c r="O1" s="48">
+      <c r="O1" s="43">
         <v>13</v>
       </c>
-      <c r="P1" s="48">
+      <c r="P1" s="43">
         <v>14</v>
       </c>
-      <c r="Q1" s="48">
+      <c r="Q1" s="43">
         <v>15</v>
       </c>
-      <c r="R1" s="48">
+      <c r="R1" s="43">
         <v>16</v>
       </c>
-      <c r="S1" s="48">
+      <c r="S1" s="43">
         <v>17</v>
       </c>
-      <c r="T1" s="48">
+      <c r="T1" s="43">
         <v>18</v>
       </c>
-      <c r="U1" s="48">
+      <c r="U1" s="43">
         <v>19</v>
       </c>
-      <c r="V1" s="48">
+      <c r="V1" s="43">
         <v>20</v>
       </c>
-      <c r="W1" s="48">
+      <c r="W1" s="43">
         <v>21</v>
       </c>
-      <c r="X1" s="48">
+      <c r="X1" s="43">
         <v>22</v>
       </c>
-      <c r="Y1" s="48">
+      <c r="Y1" s="43">
         <v>23</v>
       </c>
-      <c r="Z1" s="48">
+      <c r="Z1" s="43">
         <v>24</v>
       </c>
-      <c r="AA1" s="48">
+      <c r="AA1" s="43">
         <v>25</v>
       </c>
-      <c r="AB1" s="48">
+      <c r="AB1" s="43">
         <v>26</v>
       </c>
-      <c r="AC1" s="48">
+      <c r="AC1" s="43">
         <v>27</v>
       </c>
-      <c r="AD1" s="48">
+      <c r="AD1" s="43">
         <v>28</v>
       </c>
-      <c r="AE1" s="48">
+      <c r="AE1" s="43">
         <v>29</v>
       </c>
-      <c r="AF1" s="48">
+      <c r="AF1" s="43">
         <v>30</v>
       </c>
-      <c r="AG1" s="48">
+      <c r="AG1" s="43">
         <v>31</v>
       </c>
-      <c r="AH1" s="48">
+      <c r="AH1" s="43">
         <v>32</v>
       </c>
-      <c r="AI1" s="48">
+      <c r="AI1" s="43">
         <v>33</v>
       </c>
-      <c r="AJ1" s="48">
+      <c r="AJ1" s="43">
         <v>34</v>
       </c>
-      <c r="AK1" s="48">
+      <c r="AK1" s="43">
         <v>35</v>
       </c>
-      <c r="AL1" s="48">
+      <c r="AL1" s="43">
         <v>36</v>
       </c>
-      <c r="AM1" s="48">
+      <c r="AM1" s="43">
         <v>37</v>
       </c>
-      <c r="AN1" s="48">
+      <c r="AN1" s="43">
         <v>38</v>
       </c>
-      <c r="AO1" s="48">
+      <c r="AO1" s="43">
         <v>39</v>
       </c>
-      <c r="AP1" s="48">
+      <c r="AP1" s="43">
         <v>40</v>
       </c>
-      <c r="AQ1" s="48">
+      <c r="AQ1" s="43">
         <v>41</v>
       </c>
-      <c r="AR1" s="48">
+      <c r="AR1" s="43">
         <v>42</v>
       </c>
-      <c r="AS1" s="48">
+      <c r="AS1" s="43">
         <v>43</v>
       </c>
-      <c r="AT1" s="48">
+      <c r="AT1" s="43">
         <v>44</v>
       </c>
-      <c r="AU1" s="48">
+      <c r="AU1" s="43">
         <v>45</v>
       </c>
-      <c r="AV1" s="48">
+      <c r="AV1" s="43">
         <v>46</v>
       </c>
-      <c r="AW1" s="48">
+      <c r="AW1" s="43">
         <v>47</v>
       </c>
-      <c r="AX1" s="48">
+      <c r="AX1" s="43">
         <v>48</v>
       </c>
     </row>
@@ -10527,151 +10558,151 @@
       <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2" s="46">
+      <c r="B2" s="41">
         <v>1</v>
       </c>
-      <c r="C2" s="49">
+      <c r="C2" s="44">
         <v>33.479999999999997</v>
       </c>
-      <c r="D2" s="49">
+      <c r="D2" s="44">
         <v>33.479999999999997</v>
       </c>
-      <c r="E2" s="49">
+      <c r="E2" s="44">
         <v>33.479999999999997</v>
       </c>
-      <c r="F2" s="49">
+      <c r="F2" s="44">
         <v>33.479999999999997</v>
       </c>
-      <c r="G2" s="49">
-        <v>0</v>
-      </c>
-      <c r="H2" s="49">
-        <v>0</v>
-      </c>
-      <c r="I2" s="49">
-        <v>0</v>
-      </c>
-      <c r="J2" s="49">
-        <v>0</v>
-      </c>
-      <c r="K2" s="49">
-        <v>0</v>
-      </c>
-      <c r="L2" s="49">
-        <v>0</v>
-      </c>
-      <c r="M2" s="49">
-        <v>0</v>
-      </c>
-      <c r="N2" s="49">
-        <v>0</v>
-      </c>
-      <c r="O2" s="49">
-        <v>0</v>
-      </c>
-      <c r="P2" s="49">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="49">
-        <v>0</v>
-      </c>
-      <c r="R2" s="49">
-        <v>0</v>
-      </c>
-      <c r="S2" s="49">
-        <v>0</v>
-      </c>
-      <c r="T2" s="49">
-        <v>0</v>
-      </c>
-      <c r="U2" s="49">
-        <v>0</v>
-      </c>
-      <c r="V2" s="49">
-        <v>0</v>
-      </c>
-      <c r="W2" s="49">
+      <c r="G2" s="44">
+        <v>0</v>
+      </c>
+      <c r="H2" s="44">
+        <v>0</v>
+      </c>
+      <c r="I2" s="44">
+        <v>0</v>
+      </c>
+      <c r="J2" s="44">
+        <v>0</v>
+      </c>
+      <c r="K2" s="44">
+        <v>0</v>
+      </c>
+      <c r="L2" s="44">
+        <v>0</v>
+      </c>
+      <c r="M2" s="44">
+        <v>0</v>
+      </c>
+      <c r="N2" s="44">
+        <v>0</v>
+      </c>
+      <c r="O2" s="44">
+        <v>0</v>
+      </c>
+      <c r="P2" s="44">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="44">
+        <v>0</v>
+      </c>
+      <c r="R2" s="44">
+        <v>0</v>
+      </c>
+      <c r="S2" s="44">
+        <v>0</v>
+      </c>
+      <c r="T2" s="44">
+        <v>0</v>
+      </c>
+      <c r="U2" s="44">
+        <v>0</v>
+      </c>
+      <c r="V2" s="44">
+        <v>0</v>
+      </c>
+      <c r="W2" s="44">
         <v>33.479999999999997</v>
       </c>
-      <c r="X2" s="49">
+      <c r="X2" s="44">
         <v>33.479999999999997</v>
       </c>
-      <c r="Y2" s="49">
+      <c r="Y2" s="44">
         <v>33.479999999999997</v>
       </c>
-      <c r="Z2" s="49">
+      <c r="Z2" s="44">
         <v>33.479999999999997</v>
       </c>
-      <c r="AA2" s="49">
+      <c r="AA2" s="44">
         <v>33.479999999999997</v>
       </c>
-      <c r="AB2" s="49">
+      <c r="AB2" s="44">
         <v>33.479999999999997</v>
       </c>
-      <c r="AC2" s="49">
+      <c r="AC2" s="44">
         <v>33.479999999999997</v>
       </c>
-      <c r="AD2" s="49">
+      <c r="AD2" s="44">
         <v>33.479999999999997</v>
       </c>
-      <c r="AE2" s="49">
+      <c r="AE2" s="44">
         <v>33.479999999999997</v>
       </c>
-      <c r="AF2" s="49">
+      <c r="AF2" s="44">
         <v>33.479999999999997</v>
       </c>
-      <c r="AG2" s="49">
+      <c r="AG2" s="44">
         <v>33.479999999999997</v>
       </c>
-      <c r="AH2" s="49">
+      <c r="AH2" s="44">
         <v>33.479999999999997</v>
       </c>
-      <c r="AI2" s="49">
+      <c r="AI2" s="44">
         <v>33.479999999999997</v>
       </c>
-      <c r="AJ2" s="49">
+      <c r="AJ2" s="44">
         <v>33.479999999999997</v>
       </c>
-      <c r="AK2" s="49">
+      <c r="AK2" s="44">
         <v>33.479999999999997</v>
       </c>
-      <c r="AL2" s="49">
+      <c r="AL2" s="44">
         <v>33.479999999999997</v>
       </c>
-      <c r="AM2" s="49">
+      <c r="AM2" s="44">
         <v>33.479999999999997</v>
       </c>
-      <c r="AN2" s="49">
+      <c r="AN2" s="44">
         <v>33.479999999999997</v>
       </c>
-      <c r="AO2" s="49">
+      <c r="AO2" s="44">
         <v>33.479999999999997</v>
       </c>
-      <c r="AP2" s="49">
+      <c r="AP2" s="44">
         <v>33.479999999999997</v>
       </c>
-      <c r="AQ2" s="49">
+      <c r="AQ2" s="44">
         <v>33.479999999999997</v>
       </c>
-      <c r="AR2" s="49">
+      <c r="AR2" s="44">
         <v>33.479999999999997</v>
       </c>
-      <c r="AS2" s="49">
+      <c r="AS2" s="44">
         <v>33.479999999999997</v>
       </c>
-      <c r="AT2" s="49">
+      <c r="AT2" s="44">
         <v>33.479999999999997</v>
       </c>
-      <c r="AU2" s="49">
+      <c r="AU2" s="44">
         <v>33.479999999999997</v>
       </c>
-      <c r="AV2" s="49">
+      <c r="AV2" s="44">
         <v>33.479999999999997</v>
       </c>
-      <c r="AW2" s="49">
+      <c r="AW2" s="44">
         <v>33.479999999999997</v>
       </c>
-      <c r="AX2" s="49">
+      <c r="AX2" s="44">
         <v>33.479999999999997</v>
       </c>
     </row>
@@ -10679,7 +10710,7 @@
       <c r="A3" s="6">
         <v>1</v>
       </c>
-      <c r="B3" s="46">
+      <c r="B3" s="41">
         <v>2</v>
       </c>
       <c r="C3" s="6">
@@ -10831,7 +10862,7 @@
       <c r="A4" s="6">
         <v>1</v>
       </c>
-      <c r="B4" s="46">
+      <c r="B4" s="41">
         <v>3</v>
       </c>
       <c r="C4" s="6">
@@ -10983,7 +11014,7 @@
       <c r="A5" s="6">
         <v>2</v>
       </c>
-      <c r="B5" s="46">
+      <c r="B5" s="41">
         <v>1</v>
       </c>
       <c r="C5" s="6">
@@ -11135,7 +11166,7 @@
       <c r="A6" s="6">
         <v>2</v>
       </c>
-      <c r="B6" s="46">
+      <c r="B6" s="41">
         <v>2</v>
       </c>
       <c r="C6" s="6">
@@ -11287,7 +11318,7 @@
       <c r="A7" s="6">
         <v>2</v>
       </c>
-      <c r="B7" s="46">
+      <c r="B7" s="41">
         <v>3</v>
       </c>
       <c r="C7" s="6">
@@ -11439,7 +11470,7 @@
       <c r="A8" s="6">
         <v>3</v>
       </c>
-      <c r="B8" s="46">
+      <c r="B8" s="41">
         <v>1</v>
       </c>
       <c r="C8" s="6">
@@ -11591,7 +11622,7 @@
       <c r="A9" s="6">
         <v>3</v>
       </c>
-      <c r="B9" s="46">
+      <c r="B9" s="41">
         <v>2</v>
       </c>
       <c r="C9" s="6">
@@ -11743,7 +11774,7 @@
       <c r="A10" s="6">
         <v>3</v>
       </c>
-      <c r="B10" s="46">
+      <c r="B10" s="41">
         <v>3</v>
       </c>
       <c r="C10" s="6">
@@ -11895,7 +11926,7 @@
       <c r="A11" s="6">
         <v>4</v>
       </c>
-      <c r="B11" s="46">
+      <c r="B11" s="41">
         <v>1</v>
       </c>
       <c r="C11" s="6">
@@ -12095,7 +12126,7 @@
       <c r="A12" s="6">
         <v>4</v>
       </c>
-      <c r="B12" s="46">
+      <c r="B12" s="41">
         <v>2</v>
       </c>
       <c r="C12" s="6">
@@ -12247,7 +12278,7 @@
       <c r="A13" s="6">
         <v>4</v>
       </c>
-      <c r="B13" s="46">
+      <c r="B13" s="41">
         <v>3</v>
       </c>
       <c r="C13" s="6">
@@ -12735,12 +12766,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010074FAD0E770E69846A722597CB473E680" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1d9d48dd8293e3806cc8128788dc7591">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="90937ab4-9f3a-4840-8cd4-584cb9dae1db" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8defcec0cf3b60fb897fc7d90de816c1" ns2:_="">
     <xsd:import namespace="90937ab4-9f3a-4840-8cd4-584cb9dae1db"/>
@@ -12878,6 +12903,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -12888,15 +12919,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEDC7CA4-BC55-4665-B0C3-C553BA3B5335}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37DBC317-4159-4409-B68E-EBF6721F329A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12914,6 +12936,15 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEDC7CA4-BC55-4665-B0C3-C553BA3B5335}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2785286A-65E9-4423-9A34-AC506660010A}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Me voy a acostar
</commit_message>
<xml_diff>
--- a/Parametros_Finales.xlsx
+++ b/Parametros_Finales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pedroirarrazaval/Desktop/Modelo-Capstone/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{458BCDC4-08A0-BF4C-9C27-C4302FABCC7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B94BF2E8-A287-E449-A46C-0EEECCFD64D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12460" yWindow="500" windowWidth="16340" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2917,7 +2917,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2944,7 +2944,7 @@
         <v>93</v>
       </c>
       <c r="B2" s="6">
-        <v>4800</v>
+        <v>1923</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>27</v>
@@ -2961,7 +2961,7 @@
         <v>107</v>
       </c>
       <c r="B3" s="6">
-        <v>5000</v>
+        <v>2307</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>27</v>
@@ -2978,7 +2978,7 @@
         <v>112</v>
       </c>
       <c r="B4" s="6">
-        <v>1400</v>
+        <v>1200</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>27</v>

</xml_diff>